<commit_message>
wikipedia_ppp null to int
</commit_message>
<xml_diff>
--- a/scraping/wikipedia/wikipedia_ppp/data.xlsx
+++ b/scraping/wikipedia/wikipedia_ppp/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\scraping\wikipedia_ppp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\NAUKA\Python Nauka\data_science\scraping\wikipedia\wikipedia_ppp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3849E52D-A7D8-4AB2-8CED-4C2057C00F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFF7955-80A0-4FDB-AA67-6F9F13274544}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="225">
   <si>
     <t>Country</t>
   </si>
@@ -695,594 +695,6 @@
   </si>
   <si>
     <t>Tokelau</t>
-  </si>
-  <si>
-    <t>206,878,221</t>
-  </si>
-  <si>
-    <t>40,716,448</t>
-  </si>
-  <si>
-    <t>30,507,217</t>
-  </si>
-  <si>
-    <t>17,647,050</t>
-  </si>
-  <si>
-    <t>7,191,718</t>
-  </si>
-  <si>
-    <t>6,741,192</t>
-  </si>
-  <si>
-    <t>6,161,002</t>
-  </si>
-  <si>
-    <t>5,009,483</t>
-  </si>
-  <si>
-    <t>4,958,122</t>
-  </si>
-  <si>
-    <t>4,503,783</t>
-  </si>
-  <si>
-    <t>4,447,841</t>
-  </si>
-  <si>
-    <t>3,719,110</t>
-  </si>
-  <si>
-    <t>3,651,873</t>
-  </si>
-  <si>
-    <t>3,395,916</t>
-  </si>
-  <si>
-    <t>3,365,052</t>
-  </si>
-  <si>
-    <t>2,811,948</t>
-  </si>
-  <si>
-    <t>2,730,110</t>
-  </si>
-  <si>
-    <t>2,371,530</t>
-  </si>
-  <si>
-    <t>2,229,611</t>
-  </si>
-  <si>
-    <t>2,017,513</t>
-  </si>
-  <si>
-    <t>1,980,022</t>
-  </si>
-  <si>
-    <t>1,965,839</t>
-  </si>
-  <si>
-    <t>1,851,258</t>
-  </si>
-  <si>
-    <t>1,786,203</t>
-  </si>
-  <si>
-    <t>1,783,420</t>
-  </si>
-  <si>
-    <t>1,746,269</t>
-  </si>
-  <si>
-    <t>1,671,868</t>
-  </si>
-  <si>
-    <t>1,584,958</t>
-  </si>
-  <si>
-    <t>1,526,239</t>
-  </si>
-  <si>
-    <t>1,493,423</t>
-  </si>
-  <si>
-    <t>1,479,381</t>
-  </si>
-  <si>
-    <t>1,471,655</t>
-  </si>
-  <si>
-    <t>1,190,795</t>
-  </si>
-  <si>
-    <t>1,025,615</t>
-  </si>
-  <si>
-    <t>952,644</t>
-  </si>
-  <si>
-    <t>926,759</t>
-  </si>
-  <si>
-    <t>905,227</t>
-  </si>
-  <si>
-    <t>904,496</t>
-  </si>
-  <si>
-    <t>899,114</t>
-  </si>
-  <si>
-    <t>881,083</t>
-  </si>
-  <si>
-    <t>875,334</t>
-  </si>
-  <si>
-    <t>799,680</t>
-  </si>
-  <si>
-    <t>736,732</t>
-  </si>
-  <si>
-    <t>710,195</t>
-  </si>
-  <si>
-    <t>690,902</t>
-  </si>
-  <si>
-    <t>690,059</t>
-  </si>
-  <si>
-    <t>682,861</t>
-  </si>
-  <si>
-    <t>647,322</t>
-  </si>
-  <si>
-    <t>643,052</t>
-  </si>
-  <si>
-    <t>606,590</t>
-  </si>
-  <si>
-    <t>589,806</t>
-  </si>
-  <si>
-    <t>569,985</t>
-  </si>
-  <si>
-    <t>536,096</t>
-  </si>
-  <si>
-    <t>533,752</t>
-  </si>
-  <si>
-    <t>484,408</t>
-  </si>
-  <si>
-    <t>469,844</t>
-  </si>
-  <si>
-    <t>467,590</t>
-  </si>
-  <si>
-    <t>464,419</t>
-  </si>
-  <si>
-    <t>424,871</t>
-  </si>
-  <si>
-    <t>402,155</t>
-  </si>
-  <si>
-    <t>401,968</t>
-  </si>
-  <si>
-    <t>378,083</t>
-  </si>
-  <si>
-    <t>373,156</t>
-  </si>
-  <si>
-    <t>342,604</t>
-  </si>
-  <si>
-    <t>336,082</t>
-  </si>
-  <si>
-    <t>326,894</t>
-  </si>
-  <si>
-    <t>311,791</t>
-  </si>
-  <si>
-    <t>300,122</t>
-  </si>
-  <si>
-    <t>298,934</t>
-  </si>
-  <si>
-    <t>295,118</t>
-  </si>
-  <si>
-    <t>293,592</t>
-  </si>
-  <si>
-    <t>282,833</t>
-  </si>
-  <si>
-    <t>272,100</t>
-  </si>
-  <si>
-    <t>266,832</t>
-  </si>
-  <si>
-    <t>264,699</t>
-  </si>
-  <si>
-    <t>260,503</t>
-  </si>
-  <si>
-    <t>257,020</t>
-  </si>
-  <si>
-    <t>231,160</t>
-  </si>
-  <si>
-    <t>223,984</t>
-  </si>
-  <si>
-    <t>216,221</t>
-  </si>
-  <si>
-    <t>200,760</t>
-  </si>
-  <si>
-    <t>200,150</t>
-  </si>
-  <si>
-    <t>198,268</t>
-  </si>
-  <si>
-    <t>187,109</t>
-  </si>
-  <si>
-    <t>186,106</t>
-  </si>
-  <si>
-    <t>183,725</t>
-  </si>
-  <si>
-    <t>180,640</t>
-  </si>
-  <si>
-    <t>172,974</t>
-  </si>
-  <si>
-    <t>169,034</t>
-  </si>
-  <si>
-    <t>165,442</t>
-  </si>
-  <si>
-    <t>161,137</t>
-  </si>
-  <si>
-    <t>150,047</t>
-  </si>
-  <si>
-    <t>144,098</t>
-  </si>
-  <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>136,442</t>
-  </si>
-  <si>
-    <t>136,379</t>
-  </si>
-  <si>
-    <t>131,677</t>
-  </si>
-  <si>
-    <t>130,209</t>
-  </si>
-  <si>
-    <t>123,987</t>
-  </si>
-  <si>
-    <t>123,453</t>
-  </si>
-  <si>
-    <t>117,773</t>
-  </si>
-  <si>
-    <t>113,583</t>
-  </si>
-  <si>
-    <t>112,366</t>
-  </si>
-  <si>
-    <t>105,430</t>
-  </si>
-  <si>
-    <t>104,822</t>
-  </si>
-  <si>
-    <t>98,155</t>
-  </si>
-  <si>
-    <t>93,871</t>
-  </si>
-  <si>
-    <t>93,712</t>
-  </si>
-  <si>
-    <t>88,282</t>
-  </si>
-  <si>
-    <t>85,984</t>
-  </si>
-  <si>
-    <t>83,251</t>
-  </si>
-  <si>
-    <t>78,849</t>
-  </si>
-  <si>
-    <t>78,655</t>
-  </si>
-  <si>
-    <t>75,294</t>
-  </si>
-  <si>
-    <t>75,052</t>
-  </si>
-  <si>
-    <t>74,294</t>
-  </si>
-  <si>
-    <t>73,279</t>
-  </si>
-  <si>
-    <t>72,820</t>
-  </si>
-  <si>
-    <t>72,738</t>
-  </si>
-  <si>
-    <t>72,512</t>
-  </si>
-  <si>
-    <t>69,960</t>
-  </si>
-  <si>
-    <t>69,509</t>
-  </si>
-  <si>
-    <t>68,235</t>
-  </si>
-  <si>
-    <t>64,242</t>
-  </si>
-  <si>
-    <t>63,810</t>
-  </si>
-  <si>
-    <t>63,455</t>
-  </si>
-  <si>
-    <t>63,168</t>
-  </si>
-  <si>
-    <t>63,080</t>
-  </si>
-  <si>
-    <t>62,656</t>
-  </si>
-  <si>
-    <t>61,953</t>
-  </si>
-  <si>
-    <t>61,298</t>
-  </si>
-  <si>
-    <t>61,035</t>
-  </si>
-  <si>
-    <t>58,117</t>
-  </si>
-  <si>
-    <t>57,445</t>
-  </si>
-  <si>
-    <t>56,653</t>
-  </si>
-  <si>
-    <t>53,345</t>
-  </si>
-  <si>
-    <t>52,961</t>
-  </si>
-  <si>
-    <t>51,682</t>
-  </si>
-  <si>
-    <t>48,102</t>
-  </si>
-  <si>
-    <t>46,365</t>
-  </si>
-  <si>
-    <t>43,833</t>
-  </si>
-  <si>
-    <t>43,188</t>
-  </si>
-  <si>
-    <t>42,772</t>
-  </si>
-  <si>
-    <t>42,763</t>
-  </si>
-  <si>
-    <t>41,352</t>
-  </si>
-  <si>
-    <t>40,060</t>
-  </si>
-  <si>
-    <t>38,198</t>
-  </si>
-  <si>
-    <t>37,728</t>
-  </si>
-  <si>
-    <t>34,676</t>
-  </si>
-  <si>
-    <t>33,173</t>
-  </si>
-  <si>
-    <t>33,047</t>
-  </si>
-  <si>
-    <t>33,003</t>
-  </si>
-  <si>
-    <t>32,505</t>
-  </si>
-  <si>
-    <t>32,496</t>
-  </si>
-  <si>
-    <t>32,154</t>
-  </si>
-  <si>
-    <t>31,763</t>
-  </si>
-  <si>
-    <t>21,309</t>
-  </si>
-  <si>
-    <t>16,022</t>
-  </si>
-  <si>
-    <t>16,322</t>
-  </si>
-  <si>
-    <t>15,657</t>
-  </si>
-  <si>
-    <t>15,030</t>
-  </si>
-  <si>
-    <t>14,743</t>
-  </si>
-  <si>
-    <t>14,106</t>
-  </si>
-  <si>
-    <t>13,975</t>
-  </si>
-  <si>
-    <t>11,417</t>
-  </si>
-  <si>
-    <t>11,386</t>
-  </si>
-  <si>
-    <t>10,345</t>
-  </si>
-  <si>
-    <t>9,942</t>
-  </si>
-  <si>
-    <t>7,410</t>
-  </si>
-  <si>
-    <t>7,332</t>
-  </si>
-  <si>
-    <t>6,784</t>
-  </si>
-  <si>
-    <t>6,672</t>
-  </si>
-  <si>
-    <t>6,423</t>
-  </si>
-  <si>
-    <t>6,405</t>
-  </si>
-  <si>
-    <t>6,299</t>
-  </si>
-  <si>
-    <t>5,524</t>
-  </si>
-  <si>
-    <t>5,236</t>
-  </si>
-  <si>
-    <t>4,268</t>
-  </si>
-  <si>
-    <t>3,655</t>
-  </si>
-  <si>
-    <t>3,333</t>
-  </si>
-  <si>
-    <t>2,851</t>
-  </si>
-  <si>
-    <t>2,520</t>
-  </si>
-  <si>
-    <t>2,369</t>
-  </si>
-  <si>
-    <t>2,165</t>
-  </si>
-  <si>
-    <t>1,752</t>
-  </si>
-  <si>
-    <t>1,615</t>
-  </si>
-  <si>
-    <t>1,554</t>
-  </si>
-  <si>
-    <t>1,473</t>
-  </si>
-  <si>
-    <t>1,066</t>
-  </si>
-  <si>
-    <t>803</t>
-  </si>
-  <si>
-    <t>479</t>
-  </si>
-  <si>
-    <t>451</t>
-  </si>
-  <si>
-    <t>322</t>
-  </si>
-  <si>
-    <t>281</t>
-  </si>
-  <si>
-    <t>148</t>
-  </si>
-  <si>
-    <t>69</t>
   </si>
 </sst>
 </file>
@@ -1652,14 +1064,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="A196" sqref="A196"/>
+    <sheetView tabSelected="1" topLeftCell="A211" workbookViewId="0">
+      <selection activeCell="A225" sqref="A225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1674,1784 +1086,1700 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>225</v>
+      <c r="B2">
+        <v>206878221</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>226</v>
+      <c r="B3">
+        <v>40716448</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>227</v>
+      <c r="B4">
+        <v>30507217</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
-        <v>228</v>
+      <c r="B5">
+        <v>17647050</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
-        <v>229</v>
+      <c r="B6">
+        <v>7191718</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
-        <v>230</v>
+      <c r="B7">
+        <v>6741192</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
-        <v>231</v>
+      <c r="B8">
+        <v>6161002</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>232</v>
+      <c r="B9">
+        <v>5009483</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>233</v>
+      <c r="B10">
+        <v>4958122</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
-        <v>234</v>
+      <c r="B11">
+        <v>4503783</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>235</v>
+      <c r="B12">
+        <v>4447841</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>236</v>
+      <c r="B13">
+        <v>3719110</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
-        <v>237</v>
+      <c r="B14">
+        <v>3651873</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>238</v>
+      <c r="B15">
+        <v>3395916</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
-        <v>239</v>
+      <c r="B16">
+        <v>3365052</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
-        <v>240</v>
+      <c r="B17">
+        <v>2811948</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
-        <v>241</v>
+      <c r="B18">
+        <v>2730110</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>242</v>
+      <c r="B19">
+        <v>2371530</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>243</v>
+      <c r="B20">
+        <v>2229611</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>244</v>
+      <c r="B21">
+        <v>2017513</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>245</v>
+      <c r="B22">
+        <v>1980022</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
-        <v>246</v>
+      <c r="B23">
+        <v>1965839</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-      <c r="B24" t="s">
-        <v>247</v>
+      <c r="B24">
+        <v>1851258</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>25</v>
       </c>
-      <c r="B25" t="s">
-        <v>248</v>
+      <c r="B25">
+        <v>1786203</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
-      <c r="B26" t="s">
-        <v>249</v>
+      <c r="B26">
+        <v>1783420</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
-        <v>250</v>
+      <c r="B27">
+        <v>1746269</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
-      <c r="B28" t="s">
-        <v>251</v>
+      <c r="B28">
+        <v>1671868</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" t="s">
-        <v>252</v>
+      <c r="B29">
+        <v>1584958</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B30" t="s">
-        <v>253</v>
+      <c r="B30">
+        <v>1526239</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
-      <c r="B31" t="s">
-        <v>254</v>
+      <c r="B31">
+        <v>1493423</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>32</v>
       </c>
-      <c r="B32" t="s">
-        <v>255</v>
+      <c r="B32">
+        <v>1479381</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
-      <c r="B33" t="s">
-        <v>256</v>
+      <c r="B33">
+        <v>1471655</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>34</v>
       </c>
-      <c r="B34" t="s">
-        <v>257</v>
+      <c r="B34">
+        <v>1190795</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
-      <c r="B35" t="s">
-        <v>258</v>
+      <c r="B35">
+        <v>1025615</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
-      <c r="B36" t="s">
-        <v>259</v>
+      <c r="B36">
+        <v>952644</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
-      <c r="B37" t="s">
-        <v>260</v>
+      <c r="B37">
+        <v>926759</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>38</v>
       </c>
-      <c r="B38" t="s">
-        <v>261</v>
+      <c r="B38">
+        <v>905227</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>39</v>
       </c>
-      <c r="B39" t="s">
-        <v>262</v>
+      <c r="B39">
+        <v>904496</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>40</v>
       </c>
-      <c r="B40" t="s">
-        <v>263</v>
+      <c r="B40">
+        <v>899114</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>41</v>
       </c>
-      <c r="B41" t="s">
-        <v>264</v>
+      <c r="B41">
+        <v>881083</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B42" t="s">
-        <v>265</v>
+      <c r="B42">
+        <v>875334</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>43</v>
       </c>
-      <c r="B43" t="s">
-        <v>266</v>
+      <c r="B43">
+        <v>799680</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>44</v>
       </c>
-      <c r="B44" t="s">
-        <v>267</v>
+      <c r="B44">
+        <v>736732</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
-      <c r="B45" t="s">
-        <v>268</v>
+      <c r="B45">
+        <v>710195</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>46</v>
       </c>
-      <c r="B46" t="s">
-        <v>269</v>
+      <c r="B46">
+        <v>690902</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
-      <c r="B47" t="s">
-        <v>270</v>
+      <c r="B47">
+        <v>690059</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
-        <v>271</v>
+      <c r="B48">
+        <v>682861</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
-        <v>272</v>
+      <c r="B49">
+        <v>647322</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
-      <c r="B50" t="s">
-        <v>273</v>
+      <c r="B50">
+        <v>643052</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>51</v>
       </c>
-      <c r="B51" t="s">
-        <v>274</v>
+      <c r="B51">
+        <v>606590</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>52</v>
       </c>
-      <c r="B52" t="s">
-        <v>275</v>
+      <c r="B52">
+        <v>589806</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>53</v>
       </c>
-      <c r="B53" t="s">
-        <v>276</v>
+      <c r="B53">
+        <v>569985</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>54</v>
       </c>
-      <c r="B54" t="s">
-        <v>277</v>
+      <c r="B54">
+        <v>536096</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
-      <c r="B55" t="s">
-        <v>278</v>
+      <c r="B55">
+        <v>533752</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>56</v>
       </c>
-      <c r="B56" t="s">
-        <v>279</v>
+      <c r="B56">
+        <v>484408</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>57</v>
       </c>
-      <c r="B57" t="s">
-        <v>280</v>
+      <c r="B57">
+        <v>469844</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>58</v>
       </c>
-      <c r="B58" t="s">
-        <v>281</v>
+      <c r="B58">
+        <v>467590</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>59</v>
       </c>
-      <c r="B59" t="s">
-        <v>282</v>
+      <c r="B59">
+        <v>464419</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>60</v>
       </c>
-      <c r="B60" t="s">
-        <v>283</v>
+      <c r="B60">
+        <v>424871</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>61</v>
       </c>
-      <c r="B61" t="s">
-        <v>284</v>
+      <c r="B61">
+        <v>402155</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>62</v>
       </c>
-      <c r="B62" t="s">
-        <v>285</v>
+      <c r="B62">
+        <v>401968</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>63</v>
       </c>
-      <c r="B63" t="s">
-        <v>286</v>
+      <c r="B63">
+        <v>378083</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>64</v>
       </c>
-      <c r="B64" t="s">
-        <v>287</v>
+      <c r="B64">
+        <v>373156</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>65</v>
       </c>
-      <c r="B65" t="s">
-        <v>288</v>
+      <c r="B65">
+        <v>342604</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>66</v>
       </c>
-      <c r="B66" t="s">
-        <v>289</v>
+      <c r="B66">
+        <v>336082</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>67</v>
       </c>
-      <c r="B67" t="s">
-        <v>290</v>
+      <c r="B67">
+        <v>326894</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>68</v>
       </c>
-      <c r="B68" t="s">
-        <v>291</v>
+      <c r="B68">
+        <v>311791</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>69</v>
       </c>
-      <c r="B69" t="s">
-        <v>292</v>
+      <c r="B69">
+        <v>300122</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>70</v>
       </c>
-      <c r="B70" t="s">
-        <v>293</v>
+      <c r="B70">
+        <v>298934</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>71</v>
       </c>
-      <c r="B71" t="s">
-        <v>294</v>
+      <c r="B71">
+        <v>295118</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>72</v>
       </c>
-      <c r="B72" t="s">
-        <v>295</v>
+      <c r="B72">
+        <v>293592</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>73</v>
       </c>
-      <c r="B73" t="s">
-        <v>296</v>
+      <c r="B73">
+        <v>282833</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>74</v>
       </c>
-      <c r="B74" t="s">
-        <v>297</v>
+      <c r="B74">
+        <v>272100</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>75</v>
       </c>
-      <c r="B75" t="s">
-        <v>298</v>
+      <c r="B75">
+        <v>266832</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>76</v>
       </c>
-      <c r="B76" t="s">
-        <v>299</v>
+      <c r="B76">
+        <v>264699</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>77</v>
       </c>
-      <c r="B77" t="s">
-        <v>300</v>
+      <c r="B77">
+        <v>260503</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>78</v>
       </c>
-      <c r="B78" t="s">
-        <v>301</v>
+      <c r="B78">
+        <v>257020</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>79</v>
       </c>
-      <c r="B79" t="s">
-        <v>302</v>
+      <c r="B79">
+        <v>231160</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>80</v>
       </c>
-      <c r="B80" t="s">
-        <v>303</v>
+      <c r="B80">
+        <v>223984</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>81</v>
       </c>
-      <c r="B81" t="s">
-        <v>304</v>
+      <c r="B81">
+        <v>216221</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>82</v>
       </c>
-      <c r="B82" t="s">
-        <v>305</v>
+      <c r="B82">
+        <v>200760</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>83</v>
       </c>
-      <c r="B83" t="s">
-        <v>306</v>
+      <c r="B83">
+        <v>200150</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>84</v>
       </c>
-      <c r="B84" t="s">
-        <v>307</v>
+      <c r="B84">
+        <v>198268</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>85</v>
       </c>
-      <c r="B85" t="s">
-        <v>308</v>
+      <c r="B85">
+        <v>187109</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>86</v>
       </c>
-      <c r="B86" t="s">
-        <v>309</v>
+      <c r="B86">
+        <v>186106</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>87</v>
       </c>
-      <c r="B87" t="s">
-        <v>310</v>
+      <c r="B87">
+        <v>183725</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
-      <c r="B88" t="s">
-        <v>311</v>
+      <c r="B88">
+        <v>180640</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>89</v>
       </c>
-      <c r="B89" t="s">
-        <v>312</v>
+      <c r="B89">
+        <v>172974</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>90</v>
       </c>
-      <c r="B90" t="s">
-        <v>313</v>
+      <c r="B90">
+        <v>169034</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>91</v>
       </c>
-      <c r="B91" t="s">
-        <v>314</v>
+      <c r="B91">
+        <v>165442</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>92</v>
       </c>
-      <c r="B92" t="s">
-        <v>315</v>
+      <c r="B92">
+        <v>161137</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>93</v>
       </c>
-      <c r="B93" t="s">
-        <v>316</v>
+      <c r="B93">
+        <v>150047</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>94</v>
       </c>
-      <c r="B94" t="s">
-        <v>317</v>
+      <c r="B94">
+        <v>144098</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>95</v>
       </c>
-      <c r="B95" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>96</v>
       </c>
-      <c r="B96" t="s">
-        <v>319</v>
+      <c r="B96">
+        <v>136442</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>97</v>
       </c>
-      <c r="B97" t="s">
-        <v>320</v>
+      <c r="B97">
+        <v>136379</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>98</v>
       </c>
-      <c r="B98" t="s">
-        <v>321</v>
+      <c r="B98">
+        <v>131677</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>99</v>
       </c>
-      <c r="B99" t="s">
-        <v>322</v>
+      <c r="B99">
+        <v>130209</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>100</v>
       </c>
-      <c r="B100" t="s">
-        <v>323</v>
+      <c r="B100">
+        <v>123987</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>101</v>
       </c>
-      <c r="B101" t="s">
-        <v>324</v>
+      <c r="B101">
+        <v>123453</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>102</v>
       </c>
-      <c r="B102" t="s">
-        <v>325</v>
+      <c r="B102">
+        <v>117773</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>103</v>
       </c>
-      <c r="B103" t="s">
-        <v>326</v>
+      <c r="B103">
+        <v>113583</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>104</v>
       </c>
-      <c r="B104" t="s">
-        <v>327</v>
+      <c r="B104">
+        <v>112366</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>105</v>
       </c>
-      <c r="B105" t="s">
-        <v>328</v>
+      <c r="B105">
+        <v>105430</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>106</v>
       </c>
-      <c r="B106" t="s">
-        <v>329</v>
+      <c r="B106">
+        <v>104822</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
-      <c r="B107" t="s">
-        <v>330</v>
+      <c r="B107">
+        <v>98155</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>108</v>
       </c>
-      <c r="B108" t="s">
-        <v>331</v>
+      <c r="B108">
+        <v>93871</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>109</v>
       </c>
-      <c r="B109" t="s">
-        <v>332</v>
+      <c r="B109">
+        <v>93712</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>110</v>
       </c>
-      <c r="B110" t="s">
-        <v>333</v>
+      <c r="B110">
+        <v>88282</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>111</v>
       </c>
-      <c r="B111" t="s">
-        <v>334</v>
+      <c r="B111">
+        <v>85984</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>112</v>
       </c>
-      <c r="B112" t="s">
-        <v>335</v>
+      <c r="B112">
+        <v>83251</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>113</v>
       </c>
-      <c r="B113" t="s">
-        <v>336</v>
+      <c r="B113">
+        <v>78849</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>114</v>
       </c>
-      <c r="B114" t="s">
-        <v>337</v>
+      <c r="B114">
+        <v>78655</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>115</v>
       </c>
-      <c r="B115" t="s">
-        <v>338</v>
+      <c r="B115">
+        <v>75294</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>116</v>
       </c>
-      <c r="B116" t="s">
-        <v>339</v>
+      <c r="B116">
+        <v>75052</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>117</v>
       </c>
-      <c r="B117" t="s">
-        <v>340</v>
+      <c r="B117">
+        <v>74294</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>118</v>
       </c>
-      <c r="B118" t="s">
-        <v>341</v>
+      <c r="B118">
+        <v>73279</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>119</v>
       </c>
-      <c r="B119" t="s">
-        <v>342</v>
+      <c r="B119">
+        <v>72820</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>120</v>
       </c>
-      <c r="B120" t="s">
-        <v>343</v>
+      <c r="B120">
+        <v>72738</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>121</v>
       </c>
-      <c r="B121" t="s">
-        <v>344</v>
+      <c r="B121">
+        <v>72512</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>122</v>
       </c>
-      <c r="B122" t="s">
-        <v>345</v>
+      <c r="B122">
+        <v>69960</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>123</v>
       </c>
-      <c r="B123" t="s">
-        <v>346</v>
+      <c r="B123">
+        <v>69509</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>124</v>
       </c>
-      <c r="B124" t="s">
-        <v>347</v>
+      <c r="B124">
+        <v>68235</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>125</v>
       </c>
-      <c r="B125" t="s">
-        <v>348</v>
+      <c r="B125">
+        <v>64242</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>126</v>
       </c>
-      <c r="B126" t="s">
-        <v>349</v>
+      <c r="B126">
+        <v>63810</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>127</v>
       </c>
-      <c r="B127" t="s">
-        <v>350</v>
+      <c r="B127">
+        <v>63455</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>128</v>
       </c>
-      <c r="B128" t="s">
-        <v>351</v>
+      <c r="B128">
+        <v>63168</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>129</v>
       </c>
-      <c r="B129" t="s">
-        <v>352</v>
+      <c r="B129">
+        <v>63080</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>130</v>
       </c>
-      <c r="B130" t="s">
-        <v>353</v>
+      <c r="B130">
+        <v>62656</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>131</v>
       </c>
-      <c r="B131" t="s">
-        <v>354</v>
+      <c r="B131">
+        <v>61953</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>132</v>
       </c>
-      <c r="B132" t="s">
-        <v>355</v>
+      <c r="B132">
+        <v>61298</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>133</v>
       </c>
-      <c r="B133" t="s">
-        <v>356</v>
+      <c r="B133">
+        <v>61035</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>134</v>
       </c>
-      <c r="B134" t="s">
-        <v>357</v>
+      <c r="B134">
+        <v>58117</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>135</v>
       </c>
-      <c r="B135" t="s">
-        <v>358</v>
+      <c r="B135">
+        <v>57445</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>136</v>
       </c>
-      <c r="B136" t="s">
-        <v>359</v>
+      <c r="B136">
+        <v>56653</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>137</v>
       </c>
-      <c r="B137" t="s">
-        <v>360</v>
+      <c r="B137">
+        <v>53345</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>138</v>
       </c>
-      <c r="B138" t="s">
-        <v>361</v>
+      <c r="B138">
+        <v>52961</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>139</v>
       </c>
-      <c r="B139" t="s">
-        <v>362</v>
+      <c r="B139">
+        <v>51682</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>140</v>
       </c>
-      <c r="B140" t="s">
-        <v>363</v>
+      <c r="B140">
+        <v>48102</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>141</v>
       </c>
-      <c r="B141" t="s">
-        <v>364</v>
+      <c r="B141">
+        <v>46365</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>142</v>
       </c>
-      <c r="B142" t="s">
-        <v>365</v>
+      <c r="B142">
+        <v>43833</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>143</v>
       </c>
-      <c r="B143" t="s">
-        <v>366</v>
+      <c r="B143">
+        <v>43188</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>144</v>
       </c>
-      <c r="B144" t="s">
-        <v>367</v>
+      <c r="B144">
+        <v>42772</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>145</v>
       </c>
-      <c r="B145" t="s">
-        <v>368</v>
+      <c r="B145">
+        <v>42763</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>146</v>
       </c>
-      <c r="B146" t="s">
-        <v>369</v>
+      <c r="B146">
+        <v>41352</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>147</v>
       </c>
-      <c r="B147" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>148</v>
       </c>
-      <c r="B148" t="s">
-        <v>370</v>
+      <c r="B148">
+        <v>40060</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>149</v>
       </c>
-      <c r="B149" t="s">
-        <v>371</v>
+      <c r="B149">
+        <v>38198</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>150</v>
       </c>
-      <c r="B150" t="s">
-        <v>372</v>
+      <c r="B150">
+        <v>37728</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>151</v>
       </c>
-      <c r="B151" t="s">
-        <v>373</v>
+      <c r="B151">
+        <v>34676</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>152</v>
       </c>
-      <c r="B152" t="s">
-        <v>374</v>
+      <c r="B152">
+        <v>33173</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>153</v>
       </c>
-      <c r="B153" t="s">
-        <v>375</v>
+      <c r="B153">
+        <v>33047</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>154</v>
       </c>
-      <c r="B154" t="s">
-        <v>376</v>
+      <c r="B154">
+        <v>33003</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>155</v>
       </c>
-      <c r="B155" t="s">
-        <v>377</v>
+      <c r="B155">
+        <v>32505</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>156</v>
       </c>
-      <c r="B156" t="s">
-        <v>378</v>
+      <c r="B156">
+        <v>32496</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>157</v>
       </c>
-      <c r="B157" t="s">
-        <v>379</v>
+      <c r="B157">
+        <v>32154</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>158</v>
       </c>
-      <c r="B158" t="s">
-        <v>380</v>
+      <c r="B158">
+        <v>31763</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>159</v>
       </c>
-      <c r="B159" t="s">
-        <v>381</v>
+      <c r="B159">
+        <v>21309</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>160</v>
       </c>
-      <c r="B160" t="s">
-        <v>382</v>
+      <c r="B160">
+        <v>16022</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>161</v>
       </c>
-      <c r="B161" t="s">
-        <v>383</v>
+      <c r="B161">
+        <v>16322</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>162</v>
       </c>
-      <c r="B162" t="s">
-        <v>384</v>
+      <c r="B162">
+        <v>15657</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>163</v>
       </c>
-      <c r="B163" t="s">
-        <v>385</v>
+      <c r="B163">
+        <v>15030</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>164</v>
       </c>
-      <c r="B164" t="s">
-        <v>386</v>
+      <c r="B164">
+        <v>14743</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>165</v>
       </c>
-      <c r="B165" t="s">
-        <v>387</v>
+      <c r="B165">
+        <v>14106</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>166</v>
       </c>
-      <c r="B166" t="s">
-        <v>388</v>
+      <c r="B166">
+        <v>13975</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>167</v>
       </c>
-      <c r="B167" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>168</v>
       </c>
-      <c r="B168" t="s">
-        <v>389</v>
+      <c r="B168">
+        <v>11417</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>169</v>
       </c>
-      <c r="B169" t="s">
-        <v>390</v>
+      <c r="B169">
+        <v>11386</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>170</v>
       </c>
-      <c r="B170" t="s">
-        <v>391</v>
+      <c r="B170">
+        <v>10345</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>171</v>
       </c>
-      <c r="B171" t="s">
-        <v>392</v>
+      <c r="B171">
+        <v>9942</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>172</v>
       </c>
-      <c r="B172" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>173</v>
       </c>
-      <c r="B173" t="s">
-        <v>393</v>
+      <c r="B173">
+        <v>7410</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>174</v>
       </c>
-      <c r="B174" t="s">
-        <v>394</v>
+      <c r="B174">
+        <v>7332</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>175</v>
       </c>
-      <c r="B175" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>176</v>
       </c>
-      <c r="B176" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>177</v>
       </c>
-      <c r="B177" t="s">
-        <v>395</v>
+      <c r="B177">
+        <v>6784</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>178</v>
       </c>
-      <c r="B178" t="s">
-        <v>396</v>
+      <c r="B178">
+        <v>6672</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>179</v>
       </c>
-      <c r="B179" t="s">
-        <v>397</v>
+      <c r="B179">
+        <v>6423</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>180</v>
       </c>
-      <c r="B180" t="s">
-        <v>398</v>
+      <c r="B180">
+        <v>6405</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>181</v>
       </c>
-      <c r="B181" t="s">
-        <v>399</v>
+      <c r="B181">
+        <v>6299</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>182</v>
       </c>
-      <c r="B182" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>183</v>
       </c>
-      <c r="B183" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>184</v>
       </c>
-      <c r="B184" t="s">
-        <v>400</v>
+      <c r="B184">
+        <v>5524</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>185</v>
       </c>
-      <c r="B185" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>186</v>
       </c>
-      <c r="B186" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>187</v>
       </c>
-      <c r="B187" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>188</v>
       </c>
-      <c r="B188" t="s">
-        <v>401</v>
+      <c r="B188">
+        <v>5236</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>189</v>
       </c>
-      <c r="B189" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>190</v>
       </c>
-      <c r="B190" t="s">
-        <v>402</v>
+      <c r="B190">
+        <v>4268</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>191</v>
       </c>
-      <c r="B191" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>192</v>
       </c>
-      <c r="B192" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>193</v>
       </c>
-      <c r="B193" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>194</v>
       </c>
-      <c r="B194" t="s">
-        <v>403</v>
+      <c r="B194">
+        <v>3655</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>195</v>
       </c>
-      <c r="B195" t="s">
-        <v>404</v>
+      <c r="B195">
+        <v>3333</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>196</v>
       </c>
-      <c r="B196" t="s">
-        <v>405</v>
+      <c r="B196">
+        <v>2851</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>197</v>
       </c>
-      <c r="B197" t="s">
-        <v>406</v>
+      <c r="B197">
+        <v>2520</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>198</v>
       </c>
-      <c r="B198" t="s">
-        <v>407</v>
+      <c r="B198">
+        <v>2369</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>199</v>
       </c>
-      <c r="B199" t="s">
-        <v>408</v>
+      <c r="B199">
+        <v>2165</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>200</v>
       </c>
-      <c r="B200" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>201</v>
       </c>
-      <c r="B201" t="s">
-        <v>409</v>
+      <c r="B201">
+        <v>1752</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>202</v>
       </c>
-      <c r="B202" t="s">
-        <v>410</v>
+      <c r="B202">
+        <v>1615</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>203</v>
       </c>
-      <c r="B203" t="s">
-        <v>411</v>
+      <c r="B203">
+        <v>1554</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>204</v>
       </c>
-      <c r="B204" t="s">
-        <v>412</v>
+      <c r="B204">
+        <v>1473</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>205</v>
       </c>
-      <c r="B205" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>206</v>
       </c>
-      <c r="B206" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>207</v>
       </c>
-      <c r="B207" t="s">
-        <v>413</v>
+      <c r="B207">
+        <v>1066</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>208</v>
       </c>
-      <c r="B208" t="s">
-        <v>414</v>
+      <c r="B208">
+        <v>803</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>209</v>
       </c>
-      <c r="B209" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>210</v>
       </c>
-      <c r="B210" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>211</v>
       </c>
-      <c r="B211" t="s">
-        <v>415</v>
+      <c r="B211">
+        <v>479</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>212</v>
       </c>
-      <c r="B212" t="s">
-        <v>416</v>
+      <c r="B212">
+        <v>451</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>213</v>
       </c>
-      <c r="B213" t="s">
-        <v>417</v>
+      <c r="B213">
+        <v>322</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>214</v>
       </c>
-      <c r="B214" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>215</v>
       </c>
-      <c r="B215" t="s">
-        <v>418</v>
+      <c r="B215">
+        <v>281</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>216</v>
       </c>
-      <c r="B216" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>217</v>
       </c>
-      <c r="B217" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>218</v>
       </c>
-      <c r="B218" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>219</v>
       </c>
-      <c r="B219" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>220</v>
       </c>
-      <c r="B220" t="s">
-        <v>419</v>
+      <c r="B220">
+        <v>148</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>221</v>
       </c>
-      <c r="B221" t="s">
-        <v>420</v>
+      <c r="B221">
+        <v>69</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>222</v>
       </c>
-      <c r="B222" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>223</v>
       </c>
-      <c r="B223" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>224</v>
-      </c>
-      <c r="B224" t="s">
-        <v>318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>